<commit_message>
Adds data collected from research.
</commit_message>
<xml_diff>
--- a/CS-491/research/university-reasearch.xlsx
+++ b/CS-491/research/university-reasearch.xlsx
@@ -4,44 +4,237 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Uni" sheetId="1" r:id="rId1"/>
+    <sheet name="Course" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlcn.WorksheetConnection_universityreasearch.xlsxCourse1" hidden="1">Course[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_universityreasearch.xlsxUniversity1" hidden="1">University[]</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Course-1a19e5bc-f13a-4204-8ea7-9e2883ae1f7f" name="Course" connection="WorksheetConnection_university-reasearch.xlsx!Course"/>
+          <x15:modelTable id="University-82da92b7-c439-45a4-b459-3f68003a90c8" name="University" connection="WorksheetConnection_university-reasearch.xlsx!University"/>
+        </x15:modelTables>
+        <x15:modelRelationships>
+          <x15:modelRelationship fromTable="Course" fromColumn="University Name" toTable="University" toColumn="University Name"/>
+        </x15:modelRelationships>
+      </x15:dataModel>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="5" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" name="WorksheetConnection_university-reasearch.xlsx!Course" type="102" refreshedVersion="5" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Course-1a19e5bc-f13a-4204-8ea7-9e2883ae1f7f">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_universityreasearch.xlsxCourse1"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="3" name="WorksheetConnection_university-reasearch.xlsx!University" type="102" refreshedVersion="5" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="University-82da92b7-c439-45a4-b459-3f68003a90c8">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_universityreasearch.xlsxUniversity1"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>University Name</t>
   </si>
   <si>
-    <t>Course location</t>
-  </si>
-  <si>
-    <t>Public Access</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Strutured</t>
+    <t>Publicly Accessible</t>
+  </si>
+  <si>
+    <t>Catalog Location</t>
+  </si>
+  <si>
+    <t>Structured Data</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Difficultly?</t>
+  </si>
+  <si>
+    <t>https://my.ucf.edu/psp/IHPROD/GUEST/EMPL/h/?tab=PAPP_GUEST</t>
+  </si>
+  <si>
+    <t>University of Central Florida</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M University</t>
+  </si>
+  <si>
+    <t>Javascript, XHR requests, Capatcha</t>
+  </si>
+  <si>
+    <t>Multiple Locations</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Decentralized system with my idividual schools that handle classes differently.</t>
+  </si>
+  <si>
+    <t>Ohio State University</t>
+  </si>
+  <si>
+    <t>https://classes.osu.edu/class-search/#/</t>
+  </si>
+  <si>
+    <t>Pennsylvania State University</t>
+  </si>
+  <si>
+    <t>http://schedule.psu.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASP.Net, updated hourly, pagination, in process of updating site. </t>
+  </si>
+  <si>
+    <t>University of Texas at Austin</t>
+  </si>
+  <si>
+    <t>http://registrar.utexas.edu/schedules</t>
+  </si>
+  <si>
+    <t>Requirese a login, guest login requires lot of info.</t>
+  </si>
+  <si>
+    <t>Florida International University</t>
+  </si>
+  <si>
+    <t>Javascript, XHR requests</t>
+  </si>
+  <si>
+    <t>https://pslinks.fiu.edu/psc/cslinks/EMPLOYEE/CAMP/c/COMMUNITY_ACCESS.SSS_BROWSE_CATLG.GBL&amp;FolderPath=PORTAL_ROOT_OBJECT.HC_SSS_BROWSE_CATLG_GBL4&amp;IsFolder=false&amp;IgnoreParamTempl=FolderPath,IsFolder</t>
+  </si>
+  <si>
+    <t>Arizona State University</t>
+  </si>
+  <si>
+    <t>https://webapp4.asu.edu/catalog/classlist</t>
+  </si>
+  <si>
+    <t>Michigan State University</t>
+  </si>
+  <si>
+    <t>https://one.uf.edu/soc/</t>
+  </si>
+  <si>
+    <t>University of https://one.uf.edu/soc/</t>
+  </si>
+  <si>
+    <t>Indiana University</t>
+  </si>
+  <si>
+    <t>http://registrar.indiana.edu/calendars/current/4162.shtml</t>
+  </si>
+  <si>
+    <t>Searching by params is nearly impossible, I think</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>https://courses.harvard.edu/index.html</t>
+  </si>
+  <si>
+    <t>NO OPEN STATUS!</t>
+  </si>
+  <si>
+    <t>Cuny</t>
+  </si>
+  <si>
+    <t>https://home.cunyfirst.cuny.edu/psp/cnyepprd/GUEST/HRMS/c/COMMUNITY_ACCESS.CLASS_SEARCH.GBL?FolderPath=PORTAL_ROOT_OBJECT.HC_CLASS_SEARCH_GBL&amp;IsFolder=false&amp;IgnoreParamTempl=FolderPath%252CIsFolder</t>
+  </si>
+  <si>
+    <t>Javascript, XHR requests, unique html class names :(, tables.</t>
+  </si>
+  <si>
+    <t>https://iasext.wesleyan.edu/regprod/!wesmaps_page.html?page=search</t>
+  </si>
+  <si>
+    <t>God awful tables, but workable</t>
+  </si>
+  <si>
+    <t>Wesleyan University</t>
+  </si>
+  <si>
+    <t>Stonybrook</t>
+  </si>
+  <si>
+    <t>http://www.stonybrook.edu/commcms/registrar/registration/schedules.html</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Returns EVERTHING</t>
+  </si>
+  <si>
+    <t>Pagination</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,16 +254,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -81,6 +283,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="University" displayName="University" ref="A1:G16" totalsRowShown="0">
+  <autoFilter ref="A1:G16"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="University Name"/>
+    <tableColumn id="2" name="Catalog Location" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Publicly Accessible"/>
+    <tableColumn id="4" name="Structured Data"/>
+    <tableColumn id="5" name="Difficultly?"/>
+    <tableColumn id="6" name="Enrollment" dataDxfId="0"/>
+    <tableColumn id="7" name="Multiple Locations"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Course" displayName="Course" ref="A1:A2" totalsRowShown="0">
+  <autoFilter ref="A1:A2"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="University Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,32 +598,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>51269</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <v>44315</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44201</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>40541</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2">
+        <v>39979</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2">
+        <v>39045</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2">
+        <v>38735</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2">
+        <v>37988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3">
+        <v>49042</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2">
+        <v>46817</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2">
+        <v>21000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="2">
+        <v>278000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3224</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2">
+        <v>25272</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="F16" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" location="/"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B13" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+  <tableParts count="1">
+    <tablePart r:id="rId12"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>